<commit_message>
added Aufgabe Klassendiagramm Ammusementpark
</commit_message>
<xml_diff>
--- a/unsereZeiten.xlsx
+++ b/unsereZeiten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa/Documents/Studium/3_Theoriesemester/Tutorium/Tutorium_2024_DSKI_RV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6530552-AEE3-A249-BA87-3C3575809DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04638A9D-51E6-6F43-8C5B-7BA322ABE4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,8 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -125,11 +126,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -464,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,12 +484,12 @@
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -492,8 +497,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3">
@@ -508,8 +513,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3">
@@ -520,12 +525,12 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E21" si="0">(HOUR(C5)+MINUTE(C5)/60)-(HOUR(B5)+MINUTE(B5)/60)</f>
+        <f t="shared" ref="E5:E23" si="0">(HOUR(C5)+MINUTE(C5)/60)-(HOUR(B5)+MINUTE(B5)/60)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3">
@@ -540,8 +545,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
@@ -556,8 +561,8 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3">
@@ -572,8 +577,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3">
@@ -588,8 +593,8 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
@@ -604,8 +609,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3">
@@ -620,8 +625,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3">
@@ -636,8 +641,8 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3">
@@ -652,116 +657,166 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>45338</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>45341</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>45342</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.6875</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>45342</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E15" s="2">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E16" s="2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E17" s="2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E18" s="2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E19" s="2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="2">
-        <f>SUM(E4:E13)</f>
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E31" s="2">
+        <f>SUM(E4:E28)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
         <v>1</v>
       </c>
-      <c r="H31">
+      <c r="H33">
         <f>60*3</f>
         <v>180</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J33" t="s">
         <v>2</v>
       </c>
-      <c r="K31">
+      <c r="K33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G32" t="s">
-        <v>3</v>
-      </c>
-      <c r="H32">
+      <c r="H34">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G33" t="s">
+    <row r="35" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
         <v>4</v>
       </c>
-      <c r="H33">
-        <f>H31+H32</f>
+      <c r="H35">
+        <f>H33+H34</f>
         <v>270</v>
-      </c>
-    </row>
-    <row r="34" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="J34" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34">
-        <f>H33*K31</f>
-        <v>810</v>
-      </c>
-      <c r="M34" t="s">
-        <v>6</v>
-      </c>
-      <c r="N34" s="2">
-        <f>K36-E29</f>
-        <v>-1</v>
       </c>
     </row>
     <row r="36" spans="7:14" x14ac:dyDescent="0.2">
       <c r="J36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <f>H35*K33</f>
+        <v>1080</v>
+      </c>
+      <c r="M36" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="2">
+        <f>K38-E31</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
         <v>7</v>
       </c>
-      <c r="K36">
-        <f>K34/60</f>
-        <v>13.5</v>
+      <c r="K38">
+        <f>K36/60</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>